<commit_message>
CHanged Copy of tests
</commit_message>
<xml_diff>
--- a/Copy of Test Cases IBI Bank.xlsx
+++ b/Copy of Test Cases IBI Bank.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.1 Master Page" sheetId="1" r:id="rId1"/>
     <sheet name="1.3 Login Page" sheetId="2" r:id="rId2"/>
     <sheet name="1.7 Add Branch" sheetId="3" r:id="rId3"/>
     <sheet name="1.9 Approve or Reject Requests" sheetId="4" r:id="rId4"/>
+    <sheet name="1.11 Customer Dashboard" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="183">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -244,6 +245,9 @@
     <t>Verify if  page url redirects to login page without logging into application</t>
   </si>
   <si>
+    <t>Verify https in url for login page</t>
+  </si>
+  <si>
     <t>Verify ID in url while processing your request (Eg: auth.net ?=id=101)</t>
   </si>
   <si>
@@ -310,6 +314,9 @@
     <t>033</t>
   </si>
   <si>
+    <t>034</t>
+  </si>
+  <si>
     <t>035</t>
   </si>
   <si>
@@ -439,13 +446,127 @@
     <t>Verify if the Approve / Reject Requests is not accessible to other users other than Admin</t>
   </si>
   <si>
-    <t>Make proper maessage</t>
-  </si>
-  <si>
-    <t>No log out buttom</t>
-  </si>
-  <si>
-    <t>no drop down</t>
+    <t>Verify if the Page is styled the same as the Master Page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Request Type' is clicked a drop down appears</t>
+  </si>
+  <si>
+    <t>Verify if the Dropdown list Populates the values of ‘Account Transfer’ and ‘ Account Closure’</t>
+  </si>
+  <si>
+    <t>Verify if on selecting the Account Transfer Type in the 'Request Type' Dropdown list display the details of the Account Transfer requests pending for admin’s approval</t>
+  </si>
+  <si>
+    <t>Verify if on clicking the 'Appprove', Button the status of all the selected requests have to be changed appropriately and subsequent changes have to be made in all the concerned records in the database</t>
+  </si>
+  <si>
+    <t>Verify on clicking the 'Reject' button the status of all the selected requests have to be changed appropriately</t>
+  </si>
+  <si>
+    <t>Verify on selection of Account Closure type in the 'Request Type' dropdown list, display the details of the Account Closure requests pending for admin’s approval</t>
+  </si>
+  <si>
+    <t>Verify on clicking the "Appporve' button hen the "Account Clousure' is selected the the status of all the selected requests have to be changed appropriately and subsequent changes have to be made in all the concerned records in the database</t>
+  </si>
+  <si>
+    <t>Verify on clicking the "Reject' button hen the "Account Clousure' is selected the status of all the selected requests have to be changed appropriately</t>
+  </si>
+  <si>
+    <t>Verify id on selecting the Appropaite 'Request Type' the appropaireiate page is loaded in the Admin Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if all the Mandatory Fields are filled in </t>
+  </si>
+  <si>
+    <t>Verify on clicking the 'Approve' or ‘Reject’ button, at least one of the requests should have been selected</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Page is accessible to the Customers</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Page is accessible to the Customers through the Link Url</t>
+  </si>
+  <si>
+    <t>Verify if the 'customer Dashboard' Page is displayed after successful login of the Customer</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Pages displays information regarding the savings Accounts</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Pages displays information regarding the Customers Loan Details</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' follws the same type of styling as the Master page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Pages displays information regarding the Customers Request Details</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'Create New Account ' Page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'Create New Account ' Page and on clicking it redirects to the New Account creation page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'Create New Account ' Page and on copying the link and pasting in the Url  it redirects to the New Account creation page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'Apply for Loan' Page and on clicking it redirects to the Apply for loan page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'Apply for loan ' Page and on copying the link and pasting in the Url  it redirects to the Apply for loan page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'View Update Details' Page and on clicking it redirects to the View Update Details page</t>
+  </si>
+  <si>
+    <t>Verify if the 'Customer Dashboard' Displays the quick links for the 'View Update Details ' Page and on copying the link and pasting in the Url  it redirects to the View Update Details page</t>
+  </si>
+  <si>
+    <t>Verify if the Request Details Section of the 'Customer Dashboard' displays the Number of Approved Requests</t>
+  </si>
+  <si>
+    <t>Verify if the Request Details Section of the 'Customer Dashboard' displays the Number of Rejected Requests</t>
+  </si>
+  <si>
+    <t>Verify if the Request Details Section of the 'Customer Dashboard' displays the Number of Pending Requests</t>
+  </si>
+  <si>
+    <t>Verify on click of number of Approved Request in the Request Details section of the'Customer Dashboard' Page Redirects to the page which displays the Approved requests of the customer logged in into the system</t>
+  </si>
+  <si>
+    <t>Verify on click of number of Rejected Request in the Request Details section of the'Customer Dashboard' Page Redirects to the page which displays the Rejected requests of the customer logged in into the system</t>
+  </si>
+  <si>
+    <t>Verify on click of number of  Pending Request in the Request Details section of the'Customer Dashboard' Page Redirects to the page which displays the Pending requests of the customer logged in into the system</t>
+  </si>
+  <si>
+    <t>Verify if the Loan Details of the Customer Dashboard page displays the loan details taken by logged in customer</t>
+  </si>
+  <si>
+    <t>Verify if the Account Details Section of theb Customer Dashboard page displays the saving account details of the logged in customer(Shows the Account Balance also)</t>
+  </si>
+  <si>
+    <t>Verify on click of Mini/Detailed Statements link button, customer should be navigated to the “View Mini/Detailed Transaction” Page</t>
+  </si>
+  <si>
+    <t>Verify if the Customer Dashboard page Displays the Bank logo and the header as per the styling standards as the Master Page</t>
+  </si>
+  <si>
+    <t>Verify if the Customer Dashboard page displays the Present Date on the top right corner of the header</t>
+  </si>
+  <si>
+    <t>Verify if the Customer Dashboard page displays the Customer name  who is logged into the system on the top right corner</t>
+  </si>
+  <si>
+    <t>Verify on Clicking of the log out button of the Customer gets logged out of the system and the session gets closed</t>
+  </si>
+  <si>
+    <t>Verify on copying the log out button and pastes on the URL of the Customer gets logged out of the system and the session gets closed</t>
+  </si>
+  <si>
+    <t>Loan is in sprint 3 !</t>
   </si>
 </sst>
 </file>
@@ -504,7 +625,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,7 +675,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -642,30 +769,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -973,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,8 +1115,8 @@
       <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -1019,8 +1125,8 @@
       <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -1029,8 +1135,8 @@
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -1039,8 +1145,8 @@
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -1049,8 +1155,8 @@
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -1121,7 +1227,7 @@
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="F12" s="11"/>
       <c r="G12" s="7" t="s">
@@ -1135,7 +1241,7 @@
       <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1145,8 +1251,8 @@
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
@@ -1228,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,10 +1367,10 @@
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1274,7 +1380,7 @@
       <c r="B3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1284,7 +1390,7 @@
       <c r="B4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1294,7 +1400,7 @@
       <c r="B5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1304,27 +1410,27 @@
       <c r="B6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="F8" s="3"/>
       <c r="G8" s="2" t="s">
@@ -1332,13 +1438,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="F9" s="4"/>
       <c r="G9" s="2" t="s">
@@ -1352,7 +1458,7 @@
       <c r="B10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="F10" s="5"/>
       <c r="G10" s="2" t="s">
@@ -1366,7 +1472,7 @@
       <c r="B11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="F11" s="6"/>
       <c r="G11" s="2" t="s">
@@ -1377,20 +1483,20 @@
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1400,7 +1506,7 @@
       <c r="B14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1410,47 +1516,47 @@
       <c r="B15" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="23"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1460,7 +1566,7 @@
       <c r="B20" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="23"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1470,250 +1576,258 @@
       <c r="B21" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="23"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="14"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
-        <v>86</v>
+      <c r="A24" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
-        <v>87</v>
+      <c r="A25" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
-        <v>88</v>
+      <c r="A26" s="13" t="s">
+        <v>89</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
-        <v>89</v>
+      <c r="A27" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="23"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
-        <v>90</v>
+      <c r="A28" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
-        <v>91</v>
+      <c r="A29" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="21"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
-        <v>95</v>
+      <c r="A33" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="23"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="14"/>
     </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="14"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
-        <v>100</v>
+      <c r="A38" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="23"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="14"/>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="21"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="21"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="21"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="14"/>
     </row>
     <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="21"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="14"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="21"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="14"/>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
-        <v>107</v>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="20" t="s">
-        <v>140</v>
-      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1722,22 +1836,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" activeCellId="2" sqref="E8 E9 E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="71.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="71.21875" style="2"/>
+    <col min="4" max="4" width="29.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="71.21875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="60" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1751,180 +1866,181 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C7" s="18"/>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C11" s="18"/>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C12" s="18"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C13" s="18"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C15" s="18"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C18" s="18"/>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C19" s="18"/>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C20" s="18"/>
     </row>
@@ -1933,97 +2049,97 @@
         <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C22" s="18"/>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C23" s="18"/>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
-        <v>86</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C24" s="18"/>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
-        <v>87</v>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C25" s="18"/>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
-        <v>88</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C28" s="18"/>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C29" s="18"/>
     </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C30" s="18"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C31" s="18"/>
     </row>
@@ -2034,10 +2150,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2163,7 @@
     <col min="3" max="3" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2061,123 +2177,494 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
+      <c r="F15" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="69.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="H7" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G29" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>